<commit_message>
Incluíndo o log e teste de qualidade de dados
</commit_message>
<xml_diff>
--- a/metadado/planets_metadado_to_work.xlsx
+++ b/metadado/planets_metadado_to_work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DataOps_DE03/aula03/metadado/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DataOps_DE03/aula04_pt1/metadado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="8_{FD5A1D61-5EEC-4F52-A224-6C7B828AC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0538EC37-3959-4A0A-89B1-A7EF42BC1BF2}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{FD5A1D61-5EEC-4F52-A224-6C7B828AC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1F2C312-529F-425F-BB1F-7BBFD233216F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56E82249-3F94-4ED0-8D74-558A49E5802A}"/>
+    <workbookView xWindow="1485" yWindow="1905" windowWidth="25065" windowHeight="11475" xr2:uid="{56E82249-3F94-4ED0-8D74-558A49E5802A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G14" sqref="G14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1009,8 +1009,9 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>

</xml_diff>